<commit_message>
+ trong: I'm doing my task
</commit_message>
<xml_diff>
--- a/soft-technology/data/SE06_TaskManagement_v1.0.xlsx
+++ b/soft-technology/data/SE06_TaskManagement_v1.0.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Repos\dut-projects\soft-technology\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="13875"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="InProgress" sheetId="1" r:id="rId1"/>
@@ -105,7 +100,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -113,14 +108,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,14 +123,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -587,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -598,21 +593,21 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.75" style="15" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="37" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="47.625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -635,7 +630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -656,7 +651,7 @@
       </c>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -677,7 +672,7 @@
       </c>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -698,7 +693,7 @@
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -715,11 +710,11 @@
         <v>42429</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -740,7 +735,7 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -761,7 +756,7 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="14"/>
       <c r="C8" s="11"/>
@@ -770,7 +765,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="14"/>
       <c r="C9" s="11"/>
@@ -779,7 +774,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="14"/>
       <c r="C10" s="11"/>
@@ -788,7 +783,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="14"/>
       <c r="C11" s="11"/>
@@ -797,7 +792,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="14"/>
       <c r="C12" s="11"/>
@@ -806,7 +801,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="14"/>
       <c r="C13" s="11"/>
@@ -815,7 +810,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="14"/>
       <c r="C14" s="11"/>
@@ -824,7 +819,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="14"/>
       <c r="C15" s="11"/>
@@ -833,7 +828,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="14"/>
       <c r="C16" s="11"/>
@@ -842,7 +837,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="14"/>
       <c r="C17" s="11"/>
@@ -921,18 +916,18 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.375" customWidth="1"/>
-    <col min="4" max="4" width="7.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="7.125" customWidth="1"/>
-    <col min="7" max="7" width="48.25" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -955,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -978,49 +973,49 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>

</xml_diff>